<commit_message>
iecorrect: finished testing v1!
</commit_message>
<xml_diff>
--- a/run/output/iecorrect/iecorrect-numvarname.xlsx
+++ b/run/output/iecorrect/iecorrect-numvarname.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\iefieldkit\run\output\iecorrect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A522797-6473-47A4-BEE1-20D16CE4350F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9904F8EA-1EA8-4C76-85B4-352D5640B6E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>make</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -502,8 +505,12 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>

</xml_diff>